<commit_message>
fix: update example Mappings
</commit_message>
<xml_diff>
--- a/docs/resources/Mappings_testCohort.xlsx
+++ b/docs/resources/Mappings_testCohort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\projects\catalogue\staging_2.1_merged\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEC6235-BC89-45EA-B155-E44173A5A4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A448A655-847C-446C-AF67-A5653102868B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="12180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableMappings" sheetId="2" r:id="rId1"/>
@@ -274,10 +274,10 @@
     <t>birth_weight,birth_length</t>
   </si>
   <si>
-    <t>gest_diabetes</t>
-  </si>
-  <si>
-    <t>mother</t>
+    <t>mother,mother,household</t>
+  </si>
+  <si>
+    <t>gest_diabetes,blood_glucose,partner_in_household</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB84E76-FA31-4A6A-9BE5-8663E9D70060}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N999"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -654,7 +654,7 @@
     <col min="3" max="3" width="10.58203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.2890625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.2890625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.25" style="3" bestFit="1" customWidth="1"/>
@@ -1335,10 +1335,10 @@
         <v>80</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>76</v>

</xml_diff>